<commit_message>
[importer] Set version automagically
</commit_message>
<xml_diff>
--- a/video/tools/import/schedule_ex_de.xlsx
+++ b/video/tools/import/schedule_ex_de.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="41">
   <si>
     <t xml:space="preserve">ID</t>
   </si>
@@ -82,9 +82,6 @@
     <t xml:space="preserve">Wenn diese URL ausgefüllt ist, wird man bei Klick auf den Programmpunkt in einem neuen Tab zu dieser URL weitergeleitet.</t>
   </si>
   <si>
-    <t xml:space="preserve">Version</t>
-  </si>
-  <si>
     <t xml:space="preserve">How to fill in this spreadsheet</t>
   </si>
   <si>
@@ -95,9 +92,6 @@
   </si>
   <si>
     <t xml:space="preserve">- If a talk has multiple speakers, include both IDs, and separate them with a comma</t>
-  </si>
-  <si>
-    <t xml:space="preserve">- If you send us a new file, please take care to change the version number above in K6!</t>
   </si>
   <si>
     <t xml:space="preserve">Name</t>
@@ -192,7 +186,7 @@
       <charset val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -201,86 +195,17 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF3838"/>
-        <bgColor rgb="FFFF0000"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFF972F"/>
         <bgColor rgb="FFFF8080"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="18">
+  <borders count="9">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
       <top/>
       <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right/>
-      <top style="hair"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top style="hair"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="hair"/>
-      <top/>
-      <bottom/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right style="hair"/>
-      <top style="hair"/>
-      <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="hair"/>
-      <right/>
-      <top/>
-      <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="hair"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left/>
-      <right style="hair"/>
-      <top/>
-      <bottom style="hair"/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
@@ -365,7 +290,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="29">
+  <cellXfs count="19">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -418,16 +343,20 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
@@ -435,50 +364,6 @@
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="2" borderId="8" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="12" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="13" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="15" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="16" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="3" borderId="17" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -538,7 +423,7 @@
       <rgbColor rgb="FF99CC00"/>
       <rgbColor rgb="FFFFCC00"/>
       <rgbColor rgb="FFFF972F"/>
-      <rgbColor rgb="FFFF3838"/>
+      <rgbColor rgb="FFFF6600"/>
       <rgbColor rgb="FF666699"/>
       <rgbColor rgb="FF969696"/>
       <rgbColor rgb="FF003366"/>
@@ -575,15 +460,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N1016"/>
+  <dimension ref="A1:N1015"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="bottomLeft" activeCell="A15" activeCellId="0" sqref="A15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="15.34"/>
@@ -693,33 +578,17 @@
       <c r="I4" s="6" t="s">
         <v>18</v>
       </c>
-      <c r="J4" s="9"/>
-      <c r="K4" s="10"/>
-      <c r="L4" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C5" s="6"/>
       <c r="H5" s="8"/>
-      <c r="J5" s="12"/>
-      <c r="K5" s="13" t="s">
-        <v>19</v>
-      </c>
-      <c r="L5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H6" s="8"/>
-      <c r="J6" s="12"/>
-      <c r="K6" s="15" t="n">
-        <v>1</v>
-      </c>
-      <c r="L6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C7" s="6"/>
       <c r="H7" s="8"/>
-      <c r="J7" s="16"/>
-      <c r="K7" s="17"/>
-      <c r="L7" s="18"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H8" s="8"/>
@@ -727,62 +596,57 @@
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C9" s="6"/>
       <c r="H9" s="8"/>
-      <c r="L9" s="19"/>
-      <c r="M9" s="20"/>
-      <c r="N9" s="21"/>
+      <c r="L9" s="9"/>
+      <c r="M9" s="10"/>
+      <c r="N9" s="11"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C10" s="6"/>
       <c r="H10" s="8"/>
-      <c r="L10" s="22"/>
-      <c r="M10" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="N10" s="24"/>
+      <c r="L10" s="12"/>
+      <c r="M10" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="N10" s="14"/>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H11" s="8"/>
-      <c r="L11" s="22"/>
-      <c r="M11" s="25"/>
-      <c r="N11" s="24"/>
+      <c r="L11" s="12"/>
+      <c r="M11" s="15"/>
+      <c r="N11" s="14"/>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H12" s="8"/>
-      <c r="L12" s="22"/>
-      <c r="M12" s="25" t="s">
-        <v>21</v>
-      </c>
-      <c r="N12" s="24"/>
+      <c r="L12" s="12"/>
+      <c r="M12" s="15" t="s">
+        <v>20</v>
+      </c>
+      <c r="N12" s="14"/>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H13" s="8"/>
-      <c r="L13" s="22"/>
-      <c r="M13" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="N13" s="24"/>
+      <c r="L13" s="12"/>
+      <c r="M13" s="15" t="s">
+        <v>21</v>
+      </c>
+      <c r="N13" s="14"/>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H14" s="8"/>
-      <c r="L14" s="22"/>
-      <c r="M14" s="25" t="s">
-        <v>23</v>
-      </c>
-      <c r="N14" s="24"/>
+      <c r="L14" s="12"/>
+      <c r="M14" s="15" t="s">
+        <v>22</v>
+      </c>
+      <c r="N14" s="14"/>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H15" s="8"/>
-      <c r="L15" s="22"/>
-      <c r="M15" s="25" t="s">
-        <v>24</v>
-      </c>
-      <c r="N15" s="24"/>
+      <c r="L15" s="16"/>
+      <c r="M15" s="17"/>
+      <c r="N15" s="18"/>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H16" s="8"/>
-      <c r="L16" s="26"/>
-      <c r="M16" s="27"/>
-      <c r="N16" s="28"/>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H17" s="8"/>
@@ -3781,20 +3645,17 @@
     <row r="1015" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="H1015" s="8"/>
     </row>
-    <row r="1016" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H1016" s="8"/>
-    </row>
   </sheetData>
   <dataValidations count="3">
-    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F1:G1016" type="none">
+    <dataValidation allowBlank="false" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="F1:G1015" type="none">
       <formula1>30/12/1899</formula1>
       <formula2>30/12/1899</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H1:H1016" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="H1:H1015" type="list">
       <formula1>Rooms!$A$2:$A$414</formula1>
       <formula2>0</formula2>
     </dataValidation>
-    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E1:E1016" type="list">
+    <dataValidation allowBlank="true" operator="equal" showDropDown="false" showErrorMessage="true" showInputMessage="false" sqref="E1:E1015" type="list">
       <formula1>Tracks!$A$2:$A$377</formula1>
       <formula2>0</formula2>
     </dataValidation>
@@ -3822,7 +3683,7 @@
       <selection pane="bottomLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="21.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.14"/>
@@ -3835,10 +3696,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3846,64 +3707,64 @@
         <v>11</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="C3" s="0" t="s">
         <v>29</v>
-      </c>
-      <c r="B3" s="0" t="s">
-        <v>30</v>
-      </c>
-      <c r="C3" s="0" t="s">
-        <v>31</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="9"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="11"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E5" s="12"/>
+      <c r="F5" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="14"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E6" s="12"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="14"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E7" s="12"/>
+      <c r="F7" s="15" t="s">
         <v>32</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="G7" s="14"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="12"/>
+      <c r="F8" s="15" t="s">
         <v>33</v>
       </c>
-      <c r="E4" s="19"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="21"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E5" s="22"/>
-      <c r="F5" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="24"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E6" s="22"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="24"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E7" s="22"/>
-      <c r="F7" s="25" t="s">
-        <v>34</v>
-      </c>
-      <c r="G7" s="24"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E8" s="22"/>
-      <c r="F8" s="25" t="s">
-        <v>35</v>
-      </c>
-      <c r="G8" s="24"/>
+      <c r="G8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E9" s="26"/>
-      <c r="F9" s="27"/>
-      <c r="G9" s="28"/>
+      <c r="E9" s="16"/>
+      <c r="F9" s="17"/>
+      <c r="G9" s="18"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -3929,7 +3790,7 @@
       <selection pane="bottomLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="5.42"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="54.64"/>
@@ -3941,7 +3802,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3949,44 +3810,44 @@
         <v>12</v>
       </c>
       <c r="B2" s="0" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D4" s="9"/>
+      <c r="E4" s="10"/>
+      <c r="F4" s="11"/>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D5" s="12"/>
+      <c r="E5" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5" s="14"/>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D6" s="12"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="14"/>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D7" s="12"/>
+      <c r="E7" s="15" t="s">
+        <v>35</v>
+      </c>
+      <c r="F7" s="14"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="D8" s="12"/>
+      <c r="E8" s="15" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D4" s="19"/>
-      <c r="E4" s="20"/>
-      <c r="F4" s="21"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D5" s="22"/>
-      <c r="E5" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="F5" s="24"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D6" s="22"/>
-      <c r="E6" s="25"/>
-      <c r="F6" s="24"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D7" s="22"/>
-      <c r="E7" s="25" t="s">
-        <v>37</v>
-      </c>
-      <c r="F7" s="24"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D8" s="22"/>
-      <c r="E8" s="25" t="s">
-        <v>38</v>
-      </c>
-      <c r="F8" s="24"/>
+      <c r="F8" s="14"/>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="D9" s="26"/>
-      <c r="E9" s="27"/>
-      <c r="F9" s="28"/>
+      <c r="D9" s="16"/>
+      <c r="E9" s="17"/>
+      <c r="F9" s="18"/>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
@@ -4015,7 +3876,7 @@
       <selection pane="bottomLeft" activeCell="E26" activeCellId="0" sqref="E26"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="27.51"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="5.55"/>
@@ -4028,57 +3889,57 @@
         <v>0</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E4" s="19"/>
-      <c r="F4" s="20"/>
-      <c r="G4" s="21"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="10"/>
+      <c r="G4" s="11"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E5" s="22"/>
-      <c r="F5" s="23" t="s">
-        <v>20</v>
-      </c>
-      <c r="G5" s="24"/>
+      <c r="E5" s="12"/>
+      <c r="F5" s="13" t="s">
+        <v>19</v>
+      </c>
+      <c r="G5" s="14"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E6" s="22"/>
-      <c r="F6" s="25"/>
-      <c r="G6" s="24"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="15"/>
+      <c r="G6" s="14"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E7" s="22"/>
-      <c r="F7" s="25" t="s">
+      <c r="E7" s="12"/>
+      <c r="F7" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="G7" s="14"/>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E8" s="12"/>
+      <c r="F8" s="15" t="s">
+        <v>39</v>
+      </c>
+      <c r="G8" s="14"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E9" s="12"/>
+      <c r="F9" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="G7" s="24"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E8" s="22"/>
-      <c r="F8" s="25" t="s">
-        <v>41</v>
-      </c>
-      <c r="G8" s="24"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E9" s="22"/>
-      <c r="F9" s="25" t="s">
-        <v>42</v>
-      </c>
-      <c r="G9" s="24"/>
+      <c r="G9" s="14"/>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E10" s="26"/>
-      <c r="F10" s="27"/>
-      <c r="G10" s="28"/>
+      <c r="E10" s="16"/>
+      <c r="F10" s="17"/>
+      <c r="G10" s="18"/>
     </row>
   </sheetData>
   <dataValidations count="1">

</xml_diff>